<commit_message>
fixed the org and emp schema
</commit_message>
<xml_diff>
--- a/upload/Employee.xlsx
+++ b/upload/Employee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>empId</t>
   </si>
@@ -45,18 +45,12 @@
     <t>type</t>
   </si>
   <si>
-    <t>dateOfJoin</t>
-  </si>
-  <si>
     <t>basicSalary</t>
   </si>
   <si>
     <t>montlyGoal</t>
   </si>
   <si>
-    <t>todo</t>
-  </si>
-  <si>
     <t>addOn</t>
   </si>
   <si>
@@ -84,34 +78,22 @@
     <t>Rishi Dholkheria</t>
   </si>
   <si>
-    <t>19/2/2018</t>
-  </si>
-  <si>
     <t>samridhikotnala14@gmail.com</t>
   </si>
   <si>
     <t>HR</t>
   </si>
   <si>
-    <t>30/6/2019</t>
-  </si>
-  <si>
     <t>samridhi07414902019@msi-ggsip.org</t>
   </si>
   <si>
     <t>Junior Dev</t>
   </si>
   <si>
-    <t>26/11/2017</t>
-  </si>
-  <si>
     <t>rishi05314902019@msi-ggsip.org</t>
   </si>
   <si>
     <t>OPS</t>
-  </si>
-  <si>
-    <t>19/01/2019</t>
   </si>
 </sst>
 </file>
@@ -156,10 +138,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,18 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,119 +467,98 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>10000</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2">
-        <v>44166</v>
-      </c>
-      <c r="J2">
-        <v>10000</v>
+      <c r="I3">
+        <v>14000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3">
-        <v>14000</v>
+      <c r="I5">
+        <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="J4">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="I6">
         <v>13000</v>
       </c>
     </row>
@@ -614,5 +571,6 @@
     <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>